<commit_message>
Adicionado comentário sobre as dimensões do recipiente
</commit_message>
<xml_diff>
--- a/Resources/Excel/Medidas Iniciais.xlsx
+++ b/Resources/Excel/Medidas Iniciais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="840" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="1980" yWindow="460" windowWidth="25600" windowHeight="14420" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor de Nível (Capacitância)" sheetId="1" r:id="rId1"/>
@@ -803,11 +803,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2094190592"/>
-        <c:axId val="2094191584"/>
+        <c:axId val="2092995664"/>
+        <c:axId val="2128296160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2094190592"/>
+        <c:axId val="2092995664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,12 +864,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094191584"/>
+        <c:crossAx val="2128296160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2094191584"/>
+        <c:axId val="2128296160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094190592"/>
+        <c:crossAx val="2092995664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,11 +1232,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103424512"/>
-        <c:axId val="2103425936"/>
+        <c:axId val="-2123234128"/>
+        <c:axId val="2097577184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103424512"/>
+        <c:axId val="-2123234128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,12 +1293,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103425936"/>
+        <c:crossAx val="2097577184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103425936"/>
+        <c:axId val="2097577184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1355,7 +1355,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2103424512"/>
+        <c:crossAx val="-2123234128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1686,11 +1686,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2094019040"/>
-        <c:axId val="2094007824"/>
+        <c:axId val="-2123030032"/>
+        <c:axId val="2096335888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2094019040"/>
+        <c:axId val="-2123030032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1747,12 +1747,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094007824"/>
+        <c:crossAx val="2096335888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2094007824"/>
+        <c:axId val="2096335888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,7 +1809,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094019040"/>
+        <c:crossAx val="-2123030032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3896,8 +3896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A75" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3909,6 +3909,10 @@
       <c r="B1">
         <v>0.92</v>
       </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("{",A1,",",B1,"},")</f>
+        <v>{2,0.92},</v>
+      </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
@@ -3920,6 +3924,10 @@
       <c r="B2">
         <v>1.95</v>
       </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C65" si="0">CONCATENATE("{",A2,",",B2,"},")</f>
+        <v>{4,1.95},</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -3928,6 +3936,10 @@
       <c r="B3">
         <v>2.9</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{6,2.9},</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -3936,6 +3948,10 @@
       <c r="B4">
         <v>3.5</v>
       </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{8,3.5},</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -3944,6 +3960,10 @@
       <c r="B5">
         <v>4.0199999999999996</v>
       </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{10,4.02},</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -3952,6 +3972,10 @@
       <c r="B6">
         <v>4.8</v>
       </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{12,4.8},</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -3960,6 +3984,10 @@
       <c r="B7">
         <v>5.5</v>
       </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{14,5.5},</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -3968,6 +3996,10 @@
       <c r="B8">
         <v>6.16</v>
       </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{16,6.16},</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -3976,6 +4008,10 @@
       <c r="B9">
         <v>6.84</v>
       </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{18,6.84},</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -3984,6 +4020,10 @@
       <c r="B10">
         <v>7.41</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{20,7.41},</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -3992,6 +4032,10 @@
       <c r="B11">
         <v>8.01</v>
       </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{22,8.01},</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -4000,6 +4044,10 @@
       <c r="B12">
         <v>8.82</v>
       </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>{24,8.82},</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -4008,6 +4056,10 @@
       <c r="B13">
         <v>9.4</v>
       </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>{26,9.4},</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -4016,6 +4068,10 @@
       <c r="B14">
         <v>10.18</v>
       </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>{28,10.18},</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -4024,6 +4080,10 @@
       <c r="B15">
         <v>10.9</v>
       </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>{30,10.9},</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -4032,6 +4092,10 @@
       <c r="B16">
         <v>11.4</v>
       </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>{32,11.4},</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -4040,6 +4104,10 @@
       <c r="B17">
         <v>13.71</v>
       </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>{34,13.71},</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -4048,6 +4116,10 @@
       <c r="B18">
         <v>14.39</v>
       </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>{36,14.39},</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -4056,6 +4128,10 @@
       <c r="B19">
         <v>15.02</v>
       </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>{38,15.02},</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -4064,6 +4140,10 @@
       <c r="B20">
         <v>15.84</v>
       </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>{40,15.84},</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -4072,6 +4152,10 @@
       <c r="B21">
         <v>16.420000000000002</v>
       </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>{42,16.42},</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -4080,6 +4164,10 @@
       <c r="B22">
         <v>17.28</v>
       </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>{44,17.28},</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -4088,6 +4176,10 @@
       <c r="B23">
         <v>17.79</v>
       </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>{46,17.79},</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -4096,6 +4188,10 @@
       <c r="B24">
         <v>18.61</v>
       </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>{48,18.61},</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -4104,6 +4200,10 @@
       <c r="B25">
         <v>19.28</v>
       </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>{50,19.28},</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -4112,6 +4212,10 @@
       <c r="B26">
         <v>20.100000000000001</v>
       </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>{52,20.1},</v>
+      </c>
       <c r="D26" t="s">
         <v>0</v>
       </c>
@@ -4123,6 +4227,10 @@
       <c r="B27">
         <v>20.8</v>
       </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>{54,20.8},</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -4131,6 +4239,10 @@
       <c r="B28">
         <v>21.3</v>
       </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>{56,21.3},</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -4139,6 +4251,10 @@
       <c r="B29">
         <v>22.1</v>
       </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>{58,22.1},</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -4147,6 +4263,10 @@
       <c r="B30">
         <v>22.9</v>
       </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>{60,22.9},</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -4155,6 +4275,10 @@
       <c r="B31">
         <v>23.7</v>
       </c>
+      <c r="C31" t="str">
+        <f>CONCATENATE("{",A31,",",B31,"},")</f>
+        <v>{62,23.7},</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -4163,607 +4287,883 @@
       <c r="B32">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>{64,24.6},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>66</v>
       </c>
       <c r="B33">
         <v>25.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>{66,25.4},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>68</v>
       </c>
       <c r="B34">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>{68,26.6},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>70</v>
       </c>
       <c r="B35">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>{70,27.5},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>72</v>
       </c>
       <c r="B36">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>{72,28.4},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>74</v>
       </c>
       <c r="B37">
         <v>29.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>{74,29.1},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>76</v>
       </c>
       <c r="B38">
         <v>30.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>{76,30.4},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>78</v>
       </c>
       <c r="B39">
         <v>31.3</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>{78,31.3},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>80</v>
       </c>
       <c r="B40">
         <v>32.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>{80,32.4},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>82</v>
       </c>
       <c r="B41">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>{82,33.3},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>84</v>
       </c>
       <c r="B42">
         <v>33.799999999999997</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>{84,33.8},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>86</v>
       </c>
       <c r="B43">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>{86,33.5},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>88</v>
       </c>
       <c r="B44">
         <v>35.299999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>{88,35.3},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>90</v>
       </c>
       <c r="B45">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>{90,36},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>92</v>
       </c>
       <c r="B46">
         <v>36.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>{92,36.9},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>94</v>
       </c>
       <c r="B47">
         <v>37.799999999999997</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>{94,37.8},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>96</v>
       </c>
       <c r="B48">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>{96,38.4},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>98</v>
       </c>
       <c r="B49">
         <v>39.1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>{98,39.1},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>100</v>
       </c>
       <c r="B50">
         <v>39.799999999999997</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>{100,39.8},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>102</v>
       </c>
       <c r="B51">
         <v>40.299999999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>{102,40.3},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>104</v>
       </c>
       <c r="B52">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>{104,40.8},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>106</v>
       </c>
       <c r="B53">
         <v>41.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>{106,41.6},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>108</v>
       </c>
       <c r="B54">
         <v>42.1</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" t="str">
+        <f>CONCATENATE("{",A54,",",B54,"},")</f>
+        <v>{108,42.1},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>110</v>
       </c>
       <c r="B55">
         <v>42.6</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>{110,42.6},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>112</v>
       </c>
       <c r="B56">
         <v>43.2</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>{112,43.2},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>114</v>
       </c>
       <c r="B57">
         <v>43.7</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>{114,43.7},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>116</v>
       </c>
       <c r="B58">
         <v>44.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>{116,44.4},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>118</v>
       </c>
       <c r="B59">
         <v>44.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>{118,44.9},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>120</v>
       </c>
       <c r="B60">
         <v>45.7</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>{120,45.7},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>122</v>
       </c>
       <c r="B61">
         <v>46.1</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>{122,46.1},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>124</v>
       </c>
       <c r="B62">
         <v>47</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>{124,47},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>126</v>
       </c>
       <c r="B63">
         <v>47.5</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>{126,47.5},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>128</v>
       </c>
       <c r="B64">
         <v>48.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>{128,48.4},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>130</v>
       </c>
       <c r="B65">
         <v>48.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>{130,48.8},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>132</v>
       </c>
       <c r="B66">
         <v>49.6</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C81" si="1">CONCATENATE("{",A66,",",B66,"},")</f>
+        <v>{132,49.6},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>134</v>
       </c>
       <c r="B67">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>{134,50.4},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>136</v>
       </c>
       <c r="B68">
         <v>51.2</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>{136,51.2},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>138</v>
       </c>
       <c r="B69">
         <v>51.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>{138,51.9},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>140</v>
       </c>
       <c r="B70">
         <v>52.9</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>{140,52.9},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>142</v>
       </c>
       <c r="B71">
         <v>53.5</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>{142,53.5},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>144</v>
       </c>
       <c r="B72">
         <v>54.6</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>{144,54.6},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>146</v>
       </c>
       <c r="B73">
         <v>55.1</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>{146,55.1},</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>148</v>
       </c>
       <c r="B74">
         <v>56.2</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>{148,56.2},</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>150</v>
       </c>
       <c r="B75">
         <v>57.1</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>{150,57.1},</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>152</v>
       </c>
       <c r="B76">
         <v>57.9</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>{152,57.9},</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>154</v>
       </c>
       <c r="B77">
         <v>58.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>{154,58.5},</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>156</v>
       </c>
       <c r="B78">
         <v>59.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>{156,59.5},</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>158</v>
       </c>
       <c r="B79">
         <v>60.1</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>{158,60.1},</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>160</v>
       </c>
       <c r="B80">
         <v>61.1</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>{160,61.1},</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>162</v>
       </c>
       <c r="B81">
         <v>61.8</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>{162,61.8},</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>164</v>
       </c>
       <c r="B82">
         <v>63</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C82" t="str">
+        <f>CONCATENATE("{",A82,",",B82,"},")</f>
+        <v>{164,63},</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>166</v>
       </c>
       <c r="B83">
         <v>63.7</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C83" t="str">
+        <f t="shared" ref="C83:C93" si="2">CONCATENATE("{",A83,",",B83,"},")</f>
+        <v>{166,63.7},</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>168</v>
       </c>
       <c r="B84">
         <v>65</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C84" t="str">
+        <f t="shared" si="2"/>
+        <v>{168,65},</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>170</v>
       </c>
       <c r="B85">
         <v>66</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C85" t="str">
+        <f t="shared" si="2"/>
+        <v>{170,66},</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>172</v>
       </c>
       <c r="B86">
         <v>67.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C86" t="str">
+        <f t="shared" si="2"/>
+        <v>{172,67.5},</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>174</v>
       </c>
       <c r="B87">
         <v>68.5</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C87" t="str">
+        <f t="shared" si="2"/>
+        <v>{174,68.5},</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>176</v>
       </c>
       <c r="B88">
         <v>70</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C88" t="str">
+        <f t="shared" si="2"/>
+        <v>{176,70},</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>178</v>
       </c>
       <c r="B89">
         <v>71.3</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C89" t="str">
+        <f t="shared" si="2"/>
+        <v>{178,71.3},</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>180</v>
       </c>
       <c r="B90">
         <v>73.3</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C90" t="str">
+        <f t="shared" si="2"/>
+        <v>{180,73.3},</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>182</v>
       </c>
       <c r="B91">
         <v>75.400000000000006</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C91" t="str">
+        <f t="shared" si="2"/>
+        <v>{182,75.4},</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>184</v>
       </c>
       <c r="B92">
         <v>79.2</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C92" t="str">
+        <f t="shared" si="2"/>
+        <v>{184,79.2},</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>186</v>
       </c>
       <c r="B93">
         <v>79.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C93" t="str">
+        <f t="shared" si="2"/>
+        <v>{186,79.3},</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>188</v>
       </c>
       <c r="B94">
         <v>81.2</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C94" t="str">
+        <f>CONCATENATE("{",A94,",",B94,"},")</f>
+        <v>{188,81.2},</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>190</v>
       </c>
       <c r="B95">
         <v>86</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C95" t="str">
+        <f t="shared" ref="C95:C100" si="3">CONCATENATE("{",A95,",",B95,"},")</f>
+        <v>{190,86},</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>192</v>
       </c>
       <c r="B96">
         <v>87</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C96" t="str">
+        <f t="shared" si="3"/>
+        <v>{192,87},</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>194</v>
       </c>
       <c r="B97">
         <v>86</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C97" t="str">
+        <f t="shared" si="3"/>
+        <v>{194,86},</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>196</v>
       </c>
       <c r="B98">
         <v>89.5</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C98" t="str">
+        <f t="shared" si="3"/>
+        <v>{196,89.5},</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>198</v>
       </c>
       <c r="B99">
         <v>99.1</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C99" t="str">
+        <f t="shared" si="3"/>
+        <v>{198,99.1},</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>200</v>
       </c>
       <c r="B100">
         <v>96.3</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C100" t="str">
+        <f t="shared" si="3"/>
+        <v>{200,96.3},</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>206</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>208</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>210</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>212</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>214</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>216</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>218</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>222</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>224</v>
       </c>
@@ -4991,10 +5391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C1" sqref="C1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5002,148 +5402,220 @@
     <col min="2" max="2" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>11.3</v>
       </c>
       <c r="B1" s="1">
         <v>104.4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="str">
+        <f>CONCATENATE("{",A1,",",B1,"},")</f>
+        <v>{11.3,104.4},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>13.3</v>
       </c>
       <c r="B2" s="1">
         <v>105.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C18" si="0">CONCATENATE("{",A2,",",B2,"},")</f>
+        <v>{13.3,105.3},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>15.8</v>
       </c>
       <c r="B3" s="1">
         <v>106.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{15.8,106.2},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>18.5</v>
       </c>
       <c r="B4" s="1">
         <v>107.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{18.5,107.3},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20.9</v>
       </c>
       <c r="B5" s="1">
         <v>108.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{20.9,108.2},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>23.4</v>
       </c>
       <c r="B6" s="1">
         <v>109.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{23.4,109.2},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>25.9</v>
       </c>
       <c r="B7" s="1">
         <v>110.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{25.9,110.1},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27.7</v>
       </c>
       <c r="B8" s="1">
         <v>110.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{27.7,110.8},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>29.7</v>
       </c>
       <c r="B9" s="1">
         <v>111.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{29.7,111.5},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>31.6</v>
       </c>
       <c r="B10" s="1">
         <v>112.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{31.6,112.2},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>33.799999999999997</v>
       </c>
       <c r="B11" s="1">
         <v>113.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{33.8,113.2},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>35.6</v>
       </c>
       <c r="B12" s="1">
         <v>113.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>{35.6,113.8},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>38.700000000000003</v>
       </c>
       <c r="B13" s="1">
         <v>115</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>{38.7,115},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>41.1</v>
       </c>
       <c r="B14" s="1">
         <v>115.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>{41.1,115.8},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>42.7</v>
       </c>
       <c r="B15" s="1">
         <v>116.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>{42.7,116.4},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>45.2</v>
       </c>
       <c r="B16" s="1">
         <v>117.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>{45.2,117.2},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>49.3</v>
       </c>
       <c r="B17" s="1">
         <v>118.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>{49.3,118.9},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>50.3</v>
       </c>
       <c r="B18" s="1">
         <v>119.4</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>{50.3,119.4},</v>
       </c>
     </row>
   </sheetData>
@@ -5154,180 +5626,264 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>100</v>
       </c>
       <c r="B1">
         <v>0.41699999999999998</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="str">
+        <f>CONCATENATE("{",A1,",",B1,"},")</f>
+        <v>{100,0.417},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101</v>
       </c>
       <c r="B2">
         <v>0.499</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C21" si="0">CONCATENATE("{",A2,",",B2,"},")</f>
+        <v>{101,0.499},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>102</v>
       </c>
       <c r="B3">
         <v>0.58099999999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>{102,0.581},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>103</v>
       </c>
       <c r="B4">
         <v>0.66300000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>{103,0.663},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>104</v>
       </c>
       <c r="B5">
         <v>0.74099999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>{104,0.741},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="B6">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>{105,0.82},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>106</v>
       </c>
       <c r="B7">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>{106,0.9},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>107</v>
       </c>
       <c r="B8">
         <v>0.98099999999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>{107,0.981},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>108</v>
       </c>
       <c r="B9">
         <v>1.0589999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>{108,1.059},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>109</v>
       </c>
       <c r="B10">
         <v>1.141</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>{109,1.141},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>110</v>
       </c>
       <c r="B11">
         <v>1.2030000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>{110,1.203},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>111</v>
       </c>
       <c r="B12">
         <v>1.288</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>{111,1.288},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>112</v>
       </c>
       <c r="B13">
         <v>1.373</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>{112,1.373},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>113</v>
       </c>
       <c r="B14">
         <v>1.456</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>{113,1.456},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>114</v>
       </c>
       <c r="B15">
         <v>1.5389999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>{114,1.539},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>115</v>
       </c>
       <c r="B16">
         <v>1.619</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>{115,1.619},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>116</v>
       </c>
       <c r="B17">
         <v>1.7010000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>{116,1.701},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>117</v>
       </c>
       <c r="B18">
         <v>1.7849999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>{117,1.785},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>118</v>
       </c>
       <c r="B19">
         <v>1.8680000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="str">
+        <f>CONCATENATE("{",A19,",",B19,"},")</f>
+        <v>{118,1.868},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>119</v>
       </c>
       <c r="B20">
         <v>1.964</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>{119,1.964},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>120</v>
       </c>
       <c r="B21">
         <v>2.0499999999999998</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>{120,2.05},</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metodologia e Resultados Termometro OK
</commit_message>
<xml_diff>
--- a/Resources/Excel/Medidas Iniciais.xlsx
+++ b/Resources/Excel/Medidas Iniciais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="840" windowWidth="25605" windowHeight="14415" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="1200" yWindow="840" windowWidth="25605" windowHeight="14415" tabRatio="500" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor de Nível (Capacitância)" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>200nF</t>
   </si>
@@ -65,13 +65,16 @@
     <t>V_ft(s/ offset)</t>
   </si>
   <si>
-    <t>ºC</t>
+    <t>T (ºC)</t>
   </si>
   <si>
-    <t>R Pt100</t>
+    <t>R(T)</t>
   </si>
   <si>
-    <t>INA (V)</t>
+    <t>V_out (V)</t>
+  </si>
+  <si>
+    <t>Circuito de condicionamento completo</t>
   </si>
 </sst>
 </file>
@@ -848,11 +851,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443672512"/>
-        <c:axId val="443673688"/>
+        <c:axId val="414450256"/>
+        <c:axId val="414451040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443672512"/>
+        <c:axId val="414450256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,12 +912,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443673688"/>
+        <c:crossAx val="414451040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443673688"/>
+        <c:axId val="414451040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -971,7 +974,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443672512"/>
+        <c:crossAx val="414450256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1148,7 +1151,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>11.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13.3</c:v>
@@ -1277,11 +1280,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443674472"/>
-        <c:axId val="443677216"/>
+        <c:axId val="414440456"/>
+        <c:axId val="414445160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443674472"/>
+        <c:axId val="414440456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,12 +1341,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443677216"/>
+        <c:crossAx val="414445160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443677216"/>
+        <c:axId val="414445160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1403,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443674472"/>
+        <c:crossAx val="414440456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1731,11 +1734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443675256"/>
-        <c:axId val="443677608"/>
+        <c:axId val="414446336"/>
+        <c:axId val="414446728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443675256"/>
+        <c:axId val="414446336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1792,12 +1795,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443677608"/>
+        <c:crossAx val="414446728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443677608"/>
+        <c:axId val="414446728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1857,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443675256"/>
+        <c:crossAx val="414446336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1989,14 +1992,15 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.3692913385826777E-2"/>
-                  <c:y val="-0.16245370370370371"/>
+                  <c:x val="0.1210916447944007"/>
+                  <c:y val="-9.8306357538641004E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2084,43 +2088,43 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>7.0600000000000003E-3</c:v>
+                  <c:v>5.9500000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37359999999999999</c:v>
+                  <c:v>0.36709999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7349</c:v>
+                  <c:v>0.72460000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.089</c:v>
+                  <c:v>1.077</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4770000000000001</c:v>
+                  <c:v>1.421</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.776</c:v>
+                  <c:v>1.7609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1110000000000002</c:v>
+                  <c:v>2.0920000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.44</c:v>
+                  <c:v>2.419</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.762</c:v>
+                  <c:v>2.7389999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.077</c:v>
+                  <c:v>3.0539999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3879999999999999</c:v>
+                  <c:v>3.3620000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.6930000000000001</c:v>
+                  <c:v>3.6659999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9940000000000002</c:v>
+                  <c:v>3.9630000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,11 +2139,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="443684664"/>
-        <c:axId val="443683096"/>
+        <c:axId val="414454960"/>
+        <c:axId val="414453000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="443684664"/>
+        <c:axId val="414454960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-10"/>
@@ -2197,12 +2201,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443683096"/>
+        <c:crossAx val="414453000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="443683096"/>
+        <c:axId val="414453000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2259,7 +2263,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443684664"/>
+        <c:crossAx val="414454960"/>
         <c:crossesAt val="-10"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4571,16 +4575,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>358775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6032,10 +6036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6044,7 +6048,7 @@
     <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -6057,35 +6061,35 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.1</v>
+        <v>11.3</v>
       </c>
       <c r="B2" s="1">
         <v>104.4</v>
       </c>
       <c r="C2" s="2">
-        <f>(0.3875*A2)+100</f>
-        <v>100.03874999999999</v>
+        <f>(0.385*A2)+100</f>
+        <v>104.3505</v>
       </c>
       <c r="D2" s="2">
         <f>(0.3792*A2)+100.25</f>
-        <v>100.28792</v>
-      </c>
-      <c r="F2">
+        <v>104.53496</v>
+      </c>
+      <c r="E2" s="2">
         <f>((C2-D2)/($C$19-$C$2))*100</f>
-        <v>-1.2809150494795341</v>
-      </c>
-      <c r="G2" s="2">
-        <f>ABS(F2)</f>
-        <v>1.2809150494795341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-1.2285048285048377</v>
+      </c>
+      <c r="F2" s="2">
+        <f>ABS(E2)</f>
+        <v>1.2285048285048377</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13.3</v>
       </c>
@@ -6093,23 +6097,23 @@
         <v>105.3</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C19" si="0">(0.3875*A3)+100</f>
-        <v>105.15375</v>
+        <f t="shared" ref="C3:C19" si="0">(0.385*A3)+100</f>
+        <v>105.12050000000001</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D19" si="1">(0.3792*A3)+100.25</f>
         <v>105.29336000000001</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F19" si="2">((C3-D3)/($C$19-$C$2))*100</f>
-        <v>-0.71769695411903134</v>
-      </c>
-      <c r="G3" s="2">
-        <f t="shared" ref="G3:G19" si="3">ABS(F3)</f>
-        <v>0.71769695411903134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <f>((C3-D3)/($C$19-$C$2))*100</f>
+        <v>-1.1512487512487513</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F19" si="2">ABS(E3)</f>
+        <v>1.1512487512487513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15.8</v>
       </c>
@@ -6118,22 +6122,22 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>106.1225</v>
+        <v>106.083</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
         <v>106.24136</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="2">
+        <f>((C4-D4)/($C$19-$C$2))*100</f>
+        <v>-1.0546786546786668</v>
+      </c>
+      <c r="F4" s="2">
         <f t="shared" si="2"/>
-        <v>-0.61102686030072162</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="3"/>
-        <v>0.61102686030072162</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.0546786546786668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18.5</v>
       </c>
@@ -6142,22 +6146,22 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>107.16875</v>
+        <v>107.1225</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
         <v>107.26519999999999</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="2">
+        <f>((C5-D5)/($C$19-$C$2))*100</f>
+        <v>-0.95038295038288845</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" si="2"/>
-        <v>-0.49582315897694429</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="3"/>
-        <v>0.49582315897694429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.95038295038288845</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20.9</v>
       </c>
@@ -6166,22 +6170,22 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>108.09875</v>
+        <v>108.04649999999999</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>108.17528</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="2">
+        <f>((C6-D6)/($C$19-$C$2))*100</f>
+        <v>-0.85767565767569842</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="2"/>
-        <v>-0.39341986891147801</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="3"/>
-        <v>0.39341986891147801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.85767565767569842</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23.4</v>
       </c>
@@ -6190,22 +6194,22 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>109.0675</v>
+        <v>109.009</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
         <v>109.12327999999999</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="2">
+        <f>((C7-D7)/($C$19-$C$2))*100</f>
+        <v>-0.7611055611055193</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="2"/>
-        <v>-0.28674977509316835</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="3"/>
-        <v>0.28674977509316835</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.7611055611055193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25.9</v>
       </c>
@@ -6214,22 +6218,22 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>110.03625</v>
+        <v>109.97149999999999</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
         <v>110.07128</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="2">
+        <f>((C8-D8)/($C$19-$C$2))*100</f>
+        <v>-0.66453546453552947</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="2"/>
-        <v>-0.18007968127493168</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="3"/>
-        <v>0.18007968127493168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.66453546453552947</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27.7</v>
       </c>
@@ -6238,22 +6242,22 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>110.73375</v>
+        <v>110.6645</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
         <v>110.75384</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="2">
+        <f>((C9-D9)/($C$19-$C$2))*100</f>
+        <v>-0.59500499500494741</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="2"/>
-        <v>-0.10327721372572239</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="3"/>
-        <v>0.10327721372572239</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.59500499500494741</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>29.7</v>
       </c>
@@ -6262,22 +6266,22 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>111.50875000000001</v>
+        <v>111.4345</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
         <v>111.51223999999999</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="2">
+        <f>((C10-D10)/($C$19-$C$2))*100</f>
+        <v>-0.517748917748861</v>
+      </c>
+      <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>-1.7941138671045437E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="3"/>
-        <v>1.7941138671045437E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.517748917748861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31.6</v>
       </c>
@@ -6286,22 +6290,22 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>112.245</v>
+        <v>112.166</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
         <v>112.23272</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="2">
+        <f>((C11-D11)/($C$19-$C$2))*100</f>
+        <v>-0.44435564435566877</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>6.3128132630788106E-2</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="3"/>
-        <v>6.3128132630788106E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.44435564435566877</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>33.799999999999997</v>
       </c>
@@ -6310,22 +6314,22 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>113.0975</v>
+        <v>113.01300000000001</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
         <v>113.06695999999999</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="2">
+        <f>((C12-D12)/($C$19-$C$2))*100</f>
+        <v>-0.35937395937388844</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="2"/>
-        <v>0.1569978151908597</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="3"/>
-        <v>0.1569978151908597</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.35937395937388844</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>35.6</v>
       </c>
@@ -6334,22 +6338,22 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>113.795</v>
+        <v>113.706</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
         <v>113.74952</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="2">
+        <f>((C13-D13)/($C$19-$C$2))*100</f>
+        <v>-0.28984348984349578</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="2"/>
-        <v>0.23380028273999592</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="3"/>
-        <v>0.23380028273999592</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.28984348984349578</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>38.700000000000003</v>
       </c>
@@ -6358,22 +6362,22 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>114.99625</v>
+        <v>114.8995</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
         <v>114.92504</v>
       </c>
-      <c r="F14">
+      <c r="E14" s="2">
+        <f>((C14-D14)/($C$19-$C$2))*100</f>
+        <v>-0.1700965700965191</v>
+      </c>
+      <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>0.36607119907470875</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="3"/>
-        <v>0.36607119907470875</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.1700965700965191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>41.1</v>
       </c>
@@ -6382,22 +6386,22 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>115.92625</v>
+        <v>115.8235</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
         <v>115.83512</v>
       </c>
-      <c r="F15">
+      <c r="E15" s="2">
+        <f>((C15-D15)/($C$19-$C$2))*100</f>
+        <v>-7.7389277389328909E-2</v>
+      </c>
+      <c r="F15" s="2">
         <f t="shared" si="2"/>
-        <v>0.46847448914017498</v>
-      </c>
-      <c r="G15" s="2">
-        <f t="shared" si="3"/>
-        <v>0.46847448914017498</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7.7389277389328909E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>42.7</v>
       </c>
@@ -6406,22 +6410,22 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>116.54625</v>
+        <v>116.43950000000001</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
         <v>116.44184</v>
       </c>
-      <c r="F16">
+      <c r="E16" s="2">
+        <f>((C16-D16)/($C$19-$C$2))*100</f>
+        <v>-1.5584415584346138E-2</v>
+      </c>
+      <c r="F16" s="2">
         <f t="shared" si="2"/>
-        <v>0.53674334918391653</v>
-      </c>
-      <c r="G16" s="2">
-        <f t="shared" si="3"/>
-        <v>0.53674334918391653</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.5584415584346138E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>45.2</v>
       </c>
@@ -6430,22 +6434,22 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>117.515</v>
+        <v>117.402</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
         <v>117.38983999999999</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="2">
+        <f>((C17-D17)/($C$19-$C$2))*100</f>
+        <v>8.0985680985738315E-2</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>0.64341344300222625</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="3"/>
-        <v>0.64341344300222625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8.0985680985738315E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>49.3</v>
       </c>
@@ -6454,22 +6458,22 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>119.10374999999999</v>
+        <v>118.98050000000001</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
         <v>118.94456</v>
       </c>
-      <c r="F18">
+      <c r="E18" s="2">
+        <f>((C18-D18)/($C$19-$C$2))*100</f>
+        <v>0.23936063936071092</v>
+      </c>
+      <c r="F18" s="2">
         <f t="shared" si="2"/>
-        <v>0.81835239686413142</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="3"/>
-        <v>0.81835239686413142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.23936063936071092</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>50.3</v>
       </c>
@@ -6478,25 +6482,25 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>119.49125000000001</v>
+        <v>119.3655</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
         <v>119.32375999999999</v>
       </c>
-      <c r="F19">
+      <c r="E19" s="2">
+        <f>((C19-D19)/($C$19-$C$2))*100</f>
+        <v>0.2779886779887068</v>
+      </c>
+      <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>0.86102043439154285</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="3"/>
-        <v>0.86102043439154285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="2">
-        <f>MAX(G2:G19)</f>
-        <v>1.2809150494795341</v>
+        <v>0.2779886779887068</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="2">
+        <f>MAX(F2:F19)</f>
+        <v>1.2285048285048377</v>
       </c>
     </row>
   </sheetData>
@@ -6510,7 +6514,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6963,10 +6967,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6974,7 +6978,7 @@
     <col min="3" max="3" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -6984,148 +6988,186 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-10</v>
       </c>
-      <c r="B2" s="1">
-        <v>96.13</v>
+      <c r="B2" s="2">
+        <f>100+(0.385*A2)</f>
+        <v>96.15</v>
       </c>
       <c r="C2" s="3">
-        <v>7.0600000000000003E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5.9500000000000004E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-5</v>
       </c>
-      <c r="B3" s="1">
-        <v>98.06</v>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B15" si="0">100+(0.385*A3)</f>
+        <v>98.075000000000003</v>
       </c>
       <c r="C3" s="3">
-        <v>0.37359999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.36709999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C4" s="3">
-        <v>0.7349</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.72460000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <v>101.84</v>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>101.925</v>
       </c>
       <c r="C5" s="3">
-        <v>1.089</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
-        <v>103.88</v>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>103.85</v>
       </c>
       <c r="C6" s="3">
-        <v>1.4770000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>15</v>
       </c>
-      <c r="B7" s="1">
-        <v>105.78</v>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>105.77500000000001</v>
       </c>
       <c r="C7" s="3">
-        <v>1.776</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.7609999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20</v>
       </c>
-      <c r="B8" s="1">
-        <v>107.75</v>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>107.7</v>
       </c>
       <c r="C8" s="3">
-        <v>2.1110000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0920000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25</v>
       </c>
-      <c r="B9" s="1">
-        <v>109.69</v>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>109.625</v>
       </c>
       <c r="C9" s="3">
-        <v>2.44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
-      <c r="B10" s="1">
-        <v>111.63</v>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>111.55</v>
       </c>
       <c r="C10" s="3">
-        <v>2.762</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7389999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>35</v>
       </c>
-      <c r="B11" s="1">
-        <v>113.56</v>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>113.47499999999999</v>
       </c>
       <c r="C11" s="3">
-        <v>3.077</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0539999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40</v>
       </c>
-      <c r="B12" s="1">
-        <v>115.5</v>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>115.4</v>
       </c>
       <c r="C12" s="3">
-        <v>3.3879999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.3620000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>45</v>
       </c>
-      <c r="B13" s="1">
-        <v>117.44</v>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>117.325</v>
       </c>
       <c r="C13" s="3">
-        <v>3.6930000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.6659999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
-      <c r="B14" s="1">
-        <v>119.38</v>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>119.25</v>
       </c>
       <c r="C14" s="3">
-        <v>3.9940000000000002</v>
+        <v>3.9630000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.1</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>100.0385</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.73199999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <f>B15-B4</f>
+        <v>3.8499999999999091E-2</v>
+      </c>
+      <c r="C17" s="3">
+        <f>C15-C4</f>
+        <v>7.3999999999999622E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>